<commit_message>
NPFSm Public comments updates
Updated spreadsheet with comments resolution
Uploaded NPFSm doc with PC updates for revision by comittee
</commit_message>
<xml_diff>
--- a/FHIR-R4/ITI_Comment_Form-NPFSm_Felhofer.xlsx
+++ b/FHIR-R4/ITI_Comment_Form-NPFSm_Felhofer.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10715"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22130"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lynn/Documents/IHE/2020/ITI/FHIR R4 updates/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gregorio Canal\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EAF49A95-191C-1A4E-A098-1A2213A1F156}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62693DC6-9CAF-4480-A48F-6BA7A8BD2C23}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="27600" yWindow="460" windowWidth="30360" windowHeight="16540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Comment Form" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="138">
   <si>
     <t>Priority</t>
   </si>
@@ -1142,6 +1142,40 @@
   </si>
   <si>
     <t>It seems like content.attachment.contentType and content.format will always have the same value,  right?  Is there a reason they're encoded twice?</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>comment</t>
+  </si>
+  <si>
+    <t>Discuss</t>
+  </si>
+  <si>
+    <t>Resolved</t>
+  </si>
+  <si>
+    <t>used relationship instead of association</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I always intended an NPSFSm file for a  single Privacy Policy and if needed a BPPC template will reference more than one privacy policy file. Either way Type’s cardinality is [1..1] but it is a codeableConcept thus the coding element in it it is repetable. </t>
+  </si>
+  <si>
+    <t>see above</t>
+  </si>
+  <si>
+    <t>Reject</t>
+  </si>
+  <si>
+    <t>content.attachment.contentType holds the mime-type of the document
+content-format holds the file format defined by local domain polices</t>
+  </si>
+  <si>
+    <t>IHE has never profiled a stylesheet that’s why only WorkflowDefinition template and privacy policies have a clear mapping for masterIdentifier element</t>
+  </si>
+  <si>
+    <t>Yes it is right. Because it is th same opaque identifier of the binary resource posted.</t>
   </si>
 </sst>
 </file>
@@ -1263,7 +1297,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -1340,11 +1374,35 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1377,12 +1435,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -1401,9 +1453,30 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1419,7 +1492,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema di Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1741,62 +1814,63 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="162" zoomScaleNormal="162" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView tabSelected="1" topLeftCell="B11" zoomScale="88" zoomScaleNormal="88" workbookViewId="0">
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="71.5" customWidth="1"/>
+    <col min="2" max="2" width="71.44140625" customWidth="1"/>
     <col min="3" max="3" width="4.33203125" customWidth="1"/>
-    <col min="4" max="4" width="10.5" style="9" customWidth="1"/>
-    <col min="5" max="5" width="8.83203125" style="8"/>
+    <col min="4" max="4" width="10.44140625" style="9" customWidth="1"/>
+    <col min="5" max="5" width="8.77734375" style="8"/>
     <col min="6" max="6" width="44" customWidth="1"/>
     <col min="7" max="7" width="49.6640625" style="11" customWidth="1"/>
     <col min="8" max="8" width="7.6640625" customWidth="1"/>
-    <col min="9" max="9" width="5.5" customWidth="1"/>
+    <col min="9" max="9" width="8.5546875" customWidth="1"/>
+    <col min="10" max="10" width="26.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="19" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
+    <row r="1" spans="1:10" ht="18" x14ac:dyDescent="0.35">
+      <c r="A1" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
-    </row>
-    <row r="2" spans="1:10" ht="269.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="12" t="s">
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
+    </row>
+    <row r="2" spans="1:10" ht="269.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12"/>
-      <c r="J2" s="12"/>
-    </row>
-    <row r="3" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F3" s="16"/>
-      <c r="G3" s="16"/>
-      <c r="H3" s="16"/>
-      <c r="I3" s="16"/>
-    </row>
-    <row r="4" spans="1:10" ht="14.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="F4" s="16"/>
-      <c r="G4" s="16"/>
-      <c r="H4" s="16"/>
-      <c r="I4" s="16"/>
-    </row>
-    <row r="5" spans="1:10" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="18"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="18"/>
+      <c r="I2" s="18"/>
+      <c r="J2" s="18"/>
+    </row>
+    <row r="3" spans="1:10" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="14"/>
+    </row>
+    <row r="4" spans="1:10" ht="14.55" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F4" s="14"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="14"/>
+      <c r="I4" s="14"/>
+    </row>
+    <row r="5" spans="1:10" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
@@ -1818,19 +1892,24 @@
       <c r="G5" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="H5" s="17" t="s">
+      <c r="H5" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="I5" s="16"/>
-    </row>
-    <row r="6" spans="1:10" s="15" customFormat="1" ht="96" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I5" s="24" t="s">
+        <v>127</v>
+      </c>
+      <c r="J5" s="20" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" s="13" customFormat="1" ht="96" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
         <v>63</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="C6" s="14"/>
+      <c r="C6" s="12"/>
       <c r="D6" s="4" t="s">
         <v>67</v>
       </c>
@@ -1844,16 +1923,19 @@
       <c r="H6" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="I6" s="7"/>
-    </row>
-    <row r="7" spans="1:10" s="15" customFormat="1" ht="14" x14ac:dyDescent="0.2">
+      <c r="I6" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="J6" s="21"/>
+    </row>
+    <row r="7" spans="1:10" s="13" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
         <v>63</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="C7" s="14"/>
+      <c r="C7" s="12"/>
       <c r="D7" s="4" t="s">
         <v>70</v>
       </c>
@@ -1863,15 +1945,18 @@
       <c r="F7" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="G7" s="16" t="s">
+      <c r="G7" s="14" t="s">
         <v>71</v>
       </c>
       <c r="H7" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="I7" s="7"/>
-    </row>
-    <row r="8" spans="1:10" s="15" customFormat="1" ht="42" x14ac:dyDescent="0.2">
+      <c r="I7" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="J7" s="21"/>
+    </row>
+    <row r="8" spans="1:10" s="13" customFormat="1" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
         <v>63</v>
       </c>
@@ -1896,9 +1981,12 @@
       <c r="H8" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="I8" s="7"/>
-    </row>
-    <row r="9" spans="1:10" s="15" customFormat="1" ht="14" x14ac:dyDescent="0.2">
+      <c r="I8" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="J8" s="21"/>
+    </row>
+    <row r="9" spans="1:10" s="13" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
         <v>63</v>
       </c>
@@ -1923,9 +2011,12 @@
       <c r="H9" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="I9" s="7"/>
-    </row>
-    <row r="10" spans="1:10" s="15" customFormat="1" ht="14" x14ac:dyDescent="0.2">
+      <c r="I9" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="J9" s="21"/>
+    </row>
+    <row r="10" spans="1:10" s="13" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
         <v>63</v>
       </c>
@@ -1950,9 +2041,12 @@
       <c r="H10" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="I10" s="7"/>
-    </row>
-    <row r="11" spans="1:10" s="15" customFormat="1" ht="28" x14ac:dyDescent="0.2">
+      <c r="I10" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="J10" s="21"/>
+    </row>
+    <row r="11" spans="1:10" s="13" customFormat="1" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
         <v>63</v>
       </c>
@@ -1977,9 +2071,12 @@
       <c r="H11" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="I11" s="7"/>
-    </row>
-    <row r="12" spans="1:10" s="15" customFormat="1" ht="70" x14ac:dyDescent="0.2">
+      <c r="I11" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="J11" s="21"/>
+    </row>
+    <row r="12" spans="1:10" s="13" customFormat="1" ht="79.2" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
         <v>63</v>
       </c>
@@ -2004,9 +2101,12 @@
       <c r="H12" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="I12" s="7"/>
-    </row>
-    <row r="13" spans="1:10" s="15" customFormat="1" ht="84" x14ac:dyDescent="0.2">
+      <c r="I12" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="J12" s="21"/>
+    </row>
+    <row r="13" spans="1:10" s="13" customFormat="1" ht="79.2" x14ac:dyDescent="0.3">
       <c r="A13" s="6" t="s">
         <v>63</v>
       </c>
@@ -2022,16 +2122,21 @@
       <c r="E13" s="6">
         <v>430</v>
       </c>
-      <c r="F13" s="18" t="s">
+      <c r="F13" s="16" t="s">
         <v>82</v>
       </c>
       <c r="G13" s="6"/>
       <c r="H13" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="I13" s="7"/>
-    </row>
-    <row r="14" spans="1:10" s="15" customFormat="1" ht="42" x14ac:dyDescent="0.2">
+      <c r="I13" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="J13" s="21" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" s="13" customFormat="1" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
         <v>63</v>
       </c>
@@ -2056,9 +2161,12 @@
       <c r="H14" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="I14" s="7"/>
-    </row>
-    <row r="15" spans="1:10" s="15" customFormat="1" ht="14" x14ac:dyDescent="0.2">
+      <c r="I14" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="J14" s="21"/>
+    </row>
+    <row r="15" spans="1:10" s="13" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A15" s="6" t="s">
         <v>63</v>
       </c>
@@ -2083,9 +2191,12 @@
       <c r="H15" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="I15" s="7"/>
-    </row>
-    <row r="16" spans="1:10" s="15" customFormat="1" ht="56" x14ac:dyDescent="0.2">
+      <c r="I15" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="J15" s="21"/>
+    </row>
+    <row r="16" spans="1:10" s="13" customFormat="1" ht="66" x14ac:dyDescent="0.3">
       <c r="A16" s="6" t="s">
         <v>63</v>
       </c>
@@ -2110,9 +2221,12 @@
       <c r="H16" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="7"/>
-    </row>
-    <row r="17" spans="1:9" s="15" customFormat="1" ht="42" x14ac:dyDescent="0.15">
+      <c r="I16" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="J16" s="21"/>
+    </row>
+    <row r="17" spans="1:10" s="13" customFormat="1" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>63</v>
       </c>
@@ -2131,15 +2245,18 @@
       <c r="F17" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="G17" s="19" t="s">
+      <c r="G17" s="17" t="s">
         <v>92</v>
       </c>
       <c r="H17" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="I17" s="7"/>
-    </row>
-    <row r="18" spans="1:9" s="15" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+      <c r="I17" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="J17" s="21"/>
+    </row>
+    <row r="18" spans="1:10" s="13" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
         <v>63</v>
       </c>
@@ -2164,9 +2281,12 @@
       <c r="H18" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="I18" s="7"/>
-    </row>
-    <row r="19" spans="1:9" s="15" customFormat="1" ht="182" x14ac:dyDescent="0.2">
+      <c r="I18" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="J18" s="21"/>
+    </row>
+    <row r="19" spans="1:10" s="13" customFormat="1" ht="211.2" x14ac:dyDescent="0.3">
       <c r="A19" s="6" t="s">
         <v>63</v>
       </c>
@@ -2191,9 +2311,14 @@
       <c r="H19" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="I19" s="7"/>
-    </row>
-    <row r="20" spans="1:9" s="15" customFormat="1" ht="28" x14ac:dyDescent="0.2">
+      <c r="I19" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="J19" s="22" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" s="13" customFormat="1" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A20" s="6" t="s">
         <v>63</v>
       </c>
@@ -2218,9 +2343,14 @@
       <c r="H20" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="I20" s="7"/>
-    </row>
-    <row r="21" spans="1:9" s="15" customFormat="1" ht="42" x14ac:dyDescent="0.2">
+      <c r="I20" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="J20" s="21" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" s="13" customFormat="1" ht="82.8" x14ac:dyDescent="0.3">
       <c r="A21" s="6" t="s">
         <v>63</v>
       </c>
@@ -2237,9 +2367,14 @@
       </c>
       <c r="G21" s="6"/>
       <c r="H21" s="6"/>
-      <c r="I21" s="7"/>
-    </row>
-    <row r="22" spans="1:9" s="15" customFormat="1" ht="84" x14ac:dyDescent="0.2">
+      <c r="I21" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="J21" s="21" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" s="13" customFormat="1" ht="92.4" x14ac:dyDescent="0.3">
       <c r="A22" s="6" t="s">
         <v>63</v>
       </c>
@@ -2262,9 +2397,14 @@
       <c r="H22" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="I22" s="7"/>
-    </row>
-    <row r="23" spans="1:9" s="15" customFormat="1" ht="42" x14ac:dyDescent="0.2">
+      <c r="I22" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="J22" s="21" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" s="13" customFormat="1" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A23" s="6" t="s">
         <v>63</v>
       </c>
@@ -2289,9 +2429,12 @@
       <c r="H23" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="I23" s="7"/>
-    </row>
-    <row r="24" spans="1:9" s="15" customFormat="1" ht="14" x14ac:dyDescent="0.2">
+      <c r="I23" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="J23" s="21"/>
+    </row>
+    <row r="24" spans="1:10" s="13" customFormat="1" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A24" s="6" t="s">
         <v>63</v>
       </c>
@@ -2314,9 +2457,14 @@
       <c r="H24" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="I24" s="7"/>
-    </row>
-    <row r="25" spans="1:9" s="15" customFormat="1" ht="56" x14ac:dyDescent="0.2">
+      <c r="I24" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="J24" s="21" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" s="13" customFormat="1" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A25" s="6" t="s">
         <v>63</v>
       </c>
@@ -2341,9 +2489,12 @@
       <c r="H25" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="I25" s="7"/>
-    </row>
-    <row r="26" spans="1:9" s="15" customFormat="1" ht="28" x14ac:dyDescent="0.2">
+      <c r="I25" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="J25" s="21"/>
+    </row>
+    <row r="26" spans="1:10" s="13" customFormat="1" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A26" s="6" t="s">
         <v>63</v>
       </c>
@@ -2368,9 +2519,12 @@
       <c r="H26" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="I26" s="7"/>
-    </row>
-    <row r="27" spans="1:9" s="15" customFormat="1" ht="84" x14ac:dyDescent="0.2">
+      <c r="I26" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="J26" s="21"/>
+    </row>
+    <row r="27" spans="1:10" s="13" customFormat="1" ht="79.2" x14ac:dyDescent="0.3">
       <c r="A27" s="6" t="s">
         <v>63</v>
       </c>
@@ -2395,9 +2549,12 @@
       <c r="H27" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="I27" s="7"/>
-    </row>
-    <row r="28" spans="1:9" s="15" customFormat="1" ht="14" x14ac:dyDescent="0.2">
+      <c r="I27" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="J27" s="21"/>
+    </row>
+    <row r="28" spans="1:10" s="13" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A28" s="6" t="s">
         <v>63</v>
       </c>
@@ -2422,9 +2579,12 @@
       <c r="H28" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="I28" s="7"/>
-    </row>
-    <row r="29" spans="1:9" s="15" customFormat="1" ht="14" x14ac:dyDescent="0.2">
+      <c r="I28" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="J28" s="21"/>
+    </row>
+    <row r="29" spans="1:10" s="13" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A29" s="6" t="s">
         <v>63</v>
       </c>
@@ -2449,9 +2609,12 @@
       <c r="H29" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="I29" s="7"/>
-    </row>
-    <row r="30" spans="1:9" s="15" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+      <c r="I29" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="J29" s="21"/>
+    </row>
+    <row r="30" spans="1:10" s="13" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
         <v>63</v>
       </c>
@@ -2476,9 +2639,12 @@
       <c r="H30" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="I30" s="7"/>
-    </row>
-    <row r="31" spans="1:9" s="15" customFormat="1" ht="14" x14ac:dyDescent="0.2">
+      <c r="I30" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="J30" s="21"/>
+    </row>
+    <row r="31" spans="1:10" s="13" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A31" s="6" t="s">
         <v>63</v>
       </c>
@@ -2501,23 +2667,27 @@
       <c r="H31" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="I31" s="7"/>
-    </row>
-    <row r="32" spans="1:9" s="15" customFormat="1" ht="14" x14ac:dyDescent="0.2">
-      <c r="A32" s="14"/>
+      <c r="I31" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="J31" s="21"/>
+    </row>
+    <row r="32" spans="1:10" s="13" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="A32" s="12"/>
       <c r="B32" s="3"/>
-      <c r="C32" s="14"/>
+      <c r="C32" s="12"/>
       <c r="D32" s="4"/>
       <c r="E32" s="6"/>
       <c r="F32" s="6"/>
       <c r="G32" s="6"/>
       <c r="H32" s="6"/>
-      <c r="I32" s="7"/>
-    </row>
-    <row r="33" spans="1:9" s="15" customFormat="1" ht="14" x14ac:dyDescent="0.2">
-      <c r="A33" s="14"/>
+      <c r="I32" s="5"/>
+      <c r="J32" s="23"/>
+    </row>
+    <row r="33" spans="1:9" s="13" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="A33" s="12"/>
       <c r="B33" s="3"/>
-      <c r="C33" s="14"/>
+      <c r="C33" s="12"/>
       <c r="D33" s="4"/>
       <c r="E33" s="6"/>
       <c r="F33" s="6"/>
@@ -2525,10 +2695,10 @@
       <c r="H33" s="6"/>
       <c r="I33" s="7"/>
     </row>
-    <row r="34" spans="1:9" s="15" customFormat="1" ht="14" x14ac:dyDescent="0.2">
-      <c r="A34" s="14"/>
+    <row r="34" spans="1:9" s="13" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="A34" s="12"/>
       <c r="B34" s="3"/>
-      <c r="C34" s="14"/>
+      <c r="C34" s="12"/>
       <c r="D34" s="4"/>
       <c r="E34" s="6"/>
       <c r="F34" s="6"/>
@@ -2536,10 +2706,10 @@
       <c r="H34" s="6"/>
       <c r="I34" s="7"/>
     </row>
-    <row r="35" spans="1:9" s="15" customFormat="1" ht="14" x14ac:dyDescent="0.2">
-      <c r="A35" s="14"/>
+    <row r="35" spans="1:9" s="13" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="A35" s="12"/>
       <c r="B35" s="3"/>
-      <c r="C35" s="14"/>
+      <c r="C35" s="12"/>
       <c r="D35" s="4"/>
       <c r="E35" s="6"/>
       <c r="F35" s="6"/>
@@ -2547,10 +2717,10 @@
       <c r="H35" s="6"/>
       <c r="I35" s="7"/>
     </row>
-    <row r="36" spans="1:9" s="15" customFormat="1" ht="14" x14ac:dyDescent="0.2">
-      <c r="A36" s="14"/>
+    <row r="36" spans="1:9" s="13" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="A36" s="12"/>
       <c r="B36" s="3"/>
-      <c r="C36" s="14"/>
+      <c r="C36" s="12"/>
       <c r="D36" s="4"/>
       <c r="E36" s="6"/>
       <c r="F36" s="6"/>
@@ -2558,10 +2728,10 @@
       <c r="H36" s="6"/>
       <c r="I36" s="7"/>
     </row>
-    <row r="37" spans="1:9" s="15" customFormat="1" ht="14" x14ac:dyDescent="0.2">
-      <c r="A37" s="14"/>
+    <row r="37" spans="1:9" s="13" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="A37" s="12"/>
       <c r="B37" s="3"/>
-      <c r="C37" s="14"/>
+      <c r="C37" s="12"/>
       <c r="D37" s="4"/>
       <c r="E37" s="6"/>
       <c r="F37" s="6"/>
@@ -2569,10 +2739,10 @@
       <c r="H37" s="6"/>
       <c r="I37" s="7"/>
     </row>
-    <row r="38" spans="1:9" s="15" customFormat="1" ht="14" x14ac:dyDescent="0.2">
-      <c r="A38" s="14"/>
+    <row r="38" spans="1:9" s="13" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="A38" s="12"/>
       <c r="B38" s="3"/>
-      <c r="C38" s="14"/>
+      <c r="C38" s="12"/>
       <c r="D38" s="4"/>
       <c r="E38" s="6"/>
       <c r="F38" s="6"/>
@@ -2580,10 +2750,10 @@
       <c r="H38" s="6"/>
       <c r="I38" s="7"/>
     </row>
-    <row r="39" spans="1:9" s="15" customFormat="1" ht="14" x14ac:dyDescent="0.2">
-      <c r="A39" s="14"/>
+    <row r="39" spans="1:9" s="13" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="A39" s="12"/>
       <c r="B39" s="3"/>
-      <c r="C39" s="14"/>
+      <c r="C39" s="12"/>
       <c r="D39" s="4"/>
       <c r="E39" s="6"/>
       <c r="F39" s="6"/>
@@ -2591,10 +2761,10 @@
       <c r="H39" s="6"/>
       <c r="I39" s="7"/>
     </row>
-    <row r="40" spans="1:9" s="15" customFormat="1" ht="14" x14ac:dyDescent="0.2">
-      <c r="A40" s="14"/>
+    <row r="40" spans="1:9" s="13" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="A40" s="12"/>
       <c r="B40" s="3"/>
-      <c r="C40" s="14"/>
+      <c r="C40" s="12"/>
       <c r="D40" s="4"/>
       <c r="E40" s="6"/>
       <c r="F40" s="6"/>
@@ -2602,10 +2772,10 @@
       <c r="H40" s="6"/>
       <c r="I40" s="7"/>
     </row>
-    <row r="41" spans="1:9" s="15" customFormat="1" ht="14" x14ac:dyDescent="0.2">
-      <c r="A41" s="14"/>
+    <row r="41" spans="1:9" s="13" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="A41" s="12"/>
       <c r="B41" s="3"/>
-      <c r="C41" s="14"/>
+      <c r="C41" s="12"/>
       <c r="D41" s="4"/>
       <c r="E41" s="6"/>
       <c r="F41" s="6"/>
@@ -2613,10 +2783,10 @@
       <c r="H41" s="6"/>
       <c r="I41" s="7"/>
     </row>
-    <row r="42" spans="1:9" s="15" customFormat="1" ht="14" x14ac:dyDescent="0.2">
-      <c r="A42" s="14"/>
+    <row r="42" spans="1:9" s="13" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="A42" s="12"/>
       <c r="B42" s="3"/>
-      <c r="C42" s="14"/>
+      <c r="C42" s="12"/>
       <c r="D42" s="4"/>
       <c r="E42" s="6"/>
       <c r="F42" s="6"/>
@@ -2624,10 +2794,10 @@
       <c r="H42" s="6"/>
       <c r="I42" s="7"/>
     </row>
-    <row r="43" spans="1:9" s="15" customFormat="1" ht="14" x14ac:dyDescent="0.2">
-      <c r="A43" s="14"/>
+    <row r="43" spans="1:9" s="13" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="A43" s="12"/>
       <c r="B43" s="3"/>
-      <c r="C43" s="14"/>
+      <c r="C43" s="12"/>
       <c r="D43" s="4"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
@@ -2635,10 +2805,10 @@
       <c r="H43" s="6"/>
       <c r="I43" s="7"/>
     </row>
-    <row r="44" spans="1:9" s="15" customFormat="1" ht="14" x14ac:dyDescent="0.2">
-      <c r="A44" s="14"/>
+    <row r="44" spans="1:9" s="13" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="A44" s="12"/>
       <c r="B44" s="3"/>
-      <c r="C44" s="14"/>
+      <c r="C44" s="12"/>
       <c r="D44" s="4"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
@@ -2646,10 +2816,10 @@
       <c r="H44" s="6"/>
       <c r="I44" s="7"/>
     </row>
-    <row r="45" spans="1:9" s="15" customFormat="1" ht="14" x14ac:dyDescent="0.2">
-      <c r="A45" s="14"/>
+    <row r="45" spans="1:9" s="13" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="A45" s="12"/>
       <c r="B45" s="3"/>
-      <c r="C45" s="14"/>
+      <c r="C45" s="12"/>
       <c r="D45" s="4"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
@@ -2657,7 +2827,7 @@
       <c r="H45" s="6"/>
       <c r="I45" s="7"/>
     </row>
-    <row r="46" spans="1:9" s="15" customFormat="1" ht="14" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:9" s="13" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="D46" s="5"/>
       <c r="E46" s="7"/>
       <c r="F46" s="7"/>
@@ -2665,7 +2835,7 @@
       <c r="H46" s="7"/>
       <c r="I46" s="7"/>
     </row>
-    <row r="47" spans="1:9" s="15" customFormat="1" ht="14" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:9" s="13" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="D47" s="5"/>
       <c r="E47" s="7"/>
       <c r="F47" s="7"/>
@@ -2673,7 +2843,7 @@
       <c r="H47" s="7"/>
       <c r="I47" s="7"/>
     </row>
-    <row r="48" spans="1:9" s="15" customFormat="1" ht="14" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:9" s="13" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="D48" s="5"/>
       <c r="E48" s="7"/>
       <c r="F48" s="7"/>
@@ -2681,7 +2851,7 @@
       <c r="H48" s="7"/>
       <c r="I48" s="7"/>
     </row>
-    <row r="49" spans="4:9" s="15" customFormat="1" ht="14" x14ac:dyDescent="0.2">
+    <row r="49" spans="4:9" s="13" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="D49" s="5"/>
       <c r="E49" s="7"/>
       <c r="F49" s="7"/>
@@ -2689,7 +2859,7 @@
       <c r="H49" s="7"/>
       <c r="I49" s="7"/>
     </row>
-    <row r="50" spans="4:9" s="15" customFormat="1" ht="14" x14ac:dyDescent="0.2">
+    <row r="50" spans="4:9" s="13" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="D50" s="5"/>
       <c r="E50" s="7"/>
       <c r="F50" s="7"/>
@@ -2697,7 +2867,7 @@
       <c r="H50" s="7"/>
       <c r="I50" s="7"/>
     </row>
-    <row r="51" spans="4:9" s="15" customFormat="1" ht="14" x14ac:dyDescent="0.2">
+    <row r="51" spans="4:9" s="13" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="D51" s="5"/>
       <c r="E51" s="7"/>
       <c r="F51" s="7"/>
@@ -2705,7 +2875,7 @@
       <c r="H51" s="7"/>
       <c r="I51" s="7"/>
     </row>
-    <row r="52" spans="4:9" s="15" customFormat="1" ht="14" x14ac:dyDescent="0.2">
+    <row r="52" spans="4:9" s="13" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="D52" s="5"/>
       <c r="E52" s="7"/>
       <c r="F52" s="7"/>
@@ -2713,7 +2883,7 @@
       <c r="H52" s="7"/>
       <c r="I52" s="7"/>
     </row>
-    <row r="53" spans="4:9" s="15" customFormat="1" ht="14" x14ac:dyDescent="0.2">
+    <row r="53" spans="4:9" s="13" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="D53" s="5"/>
       <c r="E53" s="7"/>
       <c r="F53" s="7"/>
@@ -2721,7 +2891,7 @@
       <c r="H53" s="7"/>
       <c r="I53" s="7"/>
     </row>
-    <row r="54" spans="4:9" s="15" customFormat="1" ht="14" x14ac:dyDescent="0.2">
+    <row r="54" spans="4:9" s="13" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="D54" s="5"/>
       <c r="E54" s="7"/>
       <c r="F54" s="7"/>
@@ -2729,7 +2899,7 @@
       <c r="H54" s="7"/>
       <c r="I54" s="7"/>
     </row>
-    <row r="55" spans="4:9" s="15" customFormat="1" ht="14" x14ac:dyDescent="0.2">
+    <row r="55" spans="4:9" s="13" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="D55" s="5"/>
       <c r="E55" s="7"/>
       <c r="F55" s="7"/>
@@ -2737,7 +2907,7 @@
       <c r="H55" s="7"/>
       <c r="I55" s="7"/>
     </row>
-    <row r="56" spans="4:9" s="15" customFormat="1" ht="14" x14ac:dyDescent="0.2">
+    <row r="56" spans="4:9" s="13" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="D56" s="5"/>
       <c r="E56" s="7"/>
       <c r="F56" s="7"/>
@@ -2745,7 +2915,7 @@
       <c r="H56" s="7"/>
       <c r="I56" s="7"/>
     </row>
-    <row r="57" spans="4:9" s="15" customFormat="1" ht="14" x14ac:dyDescent="0.2">
+    <row r="57" spans="4:9" s="13" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="D57" s="5"/>
       <c r="E57" s="7"/>
       <c r="F57" s="7"/>
@@ -2753,7 +2923,7 @@
       <c r="H57" s="7"/>
       <c r="I57" s="7"/>
     </row>
-    <row r="58" spans="4:9" s="15" customFormat="1" ht="14" x14ac:dyDescent="0.2">
+    <row r="58" spans="4:9" s="13" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="D58" s="5"/>
       <c r="E58" s="7"/>
       <c r="F58" s="7"/>
@@ -2761,7 +2931,7 @@
       <c r="H58" s="7"/>
       <c r="I58" s="7"/>
     </row>
-    <row r="59" spans="4:9" s="15" customFormat="1" ht="14" x14ac:dyDescent="0.2">
+    <row r="59" spans="4:9" s="13" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="D59" s="5"/>
       <c r="E59" s="7"/>
       <c r="F59" s="7"/>
@@ -2769,7 +2939,7 @@
       <c r="H59" s="7"/>
       <c r="I59" s="7"/>
     </row>
-    <row r="60" spans="4:9" s="15" customFormat="1" ht="14" x14ac:dyDescent="0.2">
+    <row r="60" spans="4:9" s="13" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="D60" s="5"/>
       <c r="E60" s="7"/>
       <c r="F60" s="7"/>
@@ -2777,7 +2947,7 @@
       <c r="H60" s="7"/>
       <c r="I60" s="7"/>
     </row>
-    <row r="61" spans="4:9" s="15" customFormat="1" ht="14" x14ac:dyDescent="0.2">
+    <row r="61" spans="4:9" s="13" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="D61" s="5"/>
       <c r="E61" s="7"/>
       <c r="F61" s="7"/>
@@ -2785,7 +2955,7 @@
       <c r="H61" s="7"/>
       <c r="I61" s="7"/>
     </row>
-    <row r="62" spans="4:9" s="15" customFormat="1" ht="14" x14ac:dyDescent="0.2">
+    <row r="62" spans="4:9" s="13" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="D62" s="5"/>
       <c r="E62" s="7"/>
       <c r="F62" s="7"/>
@@ -2793,7 +2963,7 @@
       <c r="H62" s="7"/>
       <c r="I62" s="7"/>
     </row>
-    <row r="63" spans="4:9" s="15" customFormat="1" ht="14" x14ac:dyDescent="0.2">
+    <row r="63" spans="4:9" s="13" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="D63" s="5"/>
       <c r="E63" s="7"/>
       <c r="F63" s="7"/>
@@ -2801,7 +2971,7 @@
       <c r="H63" s="7"/>
       <c r="I63" s="7"/>
     </row>
-    <row r="64" spans="4:9" s="15" customFormat="1" ht="14" x14ac:dyDescent="0.2">
+    <row r="64" spans="4:9" s="13" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="D64" s="5"/>
       <c r="E64" s="7"/>
       <c r="F64" s="7"/>
@@ -2809,7 +2979,7 @@
       <c r="H64" s="7"/>
       <c r="I64" s="7"/>
     </row>
-    <row r="65" spans="4:9" s="15" customFormat="1" ht="14" x14ac:dyDescent="0.2">
+    <row r="65" spans="4:9" s="13" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="D65" s="5"/>
       <c r="E65" s="7"/>
       <c r="F65" s="7"/>
@@ -2817,7 +2987,7 @@
       <c r="H65" s="7"/>
       <c r="I65" s="7"/>
     </row>
-    <row r="66" spans="4:9" s="15" customFormat="1" ht="14" x14ac:dyDescent="0.2">
+    <row r="66" spans="4:9" s="13" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="D66" s="5"/>
       <c r="E66" s="7"/>
       <c r="F66" s="7"/>
@@ -2825,7 +2995,7 @@
       <c r="H66" s="7"/>
       <c r="I66" s="7"/>
     </row>
-    <row r="67" spans="4:9" s="15" customFormat="1" ht="14" x14ac:dyDescent="0.2">
+    <row r="67" spans="4:9" s="13" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="D67" s="5"/>
       <c r="E67" s="7"/>
       <c r="F67" s="7"/>
@@ -2833,7 +3003,7 @@
       <c r="H67" s="7"/>
       <c r="I67" s="7"/>
     </row>
-    <row r="68" spans="4:9" s="15" customFormat="1" ht="14" x14ac:dyDescent="0.2">
+    <row r="68" spans="4:9" s="13" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="D68" s="5"/>
       <c r="E68" s="7"/>
       <c r="F68" s="7"/>
@@ -2841,7 +3011,7 @@
       <c r="H68" s="7"/>
       <c r="I68" s="7"/>
     </row>
-    <row r="69" spans="4:9" s="15" customFormat="1" ht="14" x14ac:dyDescent="0.2">
+    <row r="69" spans="4:9" s="13" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="D69" s="5"/>
       <c r="E69" s="7"/>
       <c r="F69" s="7"/>
@@ -2849,7 +3019,7 @@
       <c r="H69" s="7"/>
       <c r="I69" s="7"/>
     </row>
-    <row r="70" spans="4:9" s="15" customFormat="1" ht="14" x14ac:dyDescent="0.2">
+    <row r="70" spans="4:9" s="13" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="D70" s="5"/>
       <c r="E70" s="7"/>
       <c r="F70" s="7"/>
@@ -2857,7 +3027,7 @@
       <c r="H70" s="7"/>
       <c r="I70" s="7"/>
     </row>
-    <row r="71" spans="4:9" s="15" customFormat="1" ht="14" x14ac:dyDescent="0.2">
+    <row r="71" spans="4:9" s="13" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="D71" s="5"/>
       <c r="E71" s="7"/>
       <c r="F71" s="7"/>
@@ -2865,7 +3035,7 @@
       <c r="H71" s="7"/>
       <c r="I71" s="7"/>
     </row>
-    <row r="72" spans="4:9" s="15" customFormat="1" ht="14" x14ac:dyDescent="0.2">
+    <row r="72" spans="4:9" s="13" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="D72" s="5"/>
       <c r="E72" s="7"/>
       <c r="F72" s="7"/>
@@ -2873,83 +3043,83 @@
       <c r="H72" s="7"/>
       <c r="I72" s="7"/>
     </row>
-    <row r="73" spans="4:9" s="15" customFormat="1" ht="14" x14ac:dyDescent="0.2">
+    <row r="73" spans="4:9" s="13" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="D73" s="5"/>
       <c r="E73" s="7"/>
     </row>
-    <row r="74" spans="4:9" s="15" customFormat="1" ht="14" x14ac:dyDescent="0.2">
+    <row r="74" spans="4:9" s="13" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="D74" s="5"/>
       <c r="E74" s="7"/>
     </row>
-    <row r="75" spans="4:9" s="15" customFormat="1" ht="14" x14ac:dyDescent="0.2">
+    <row r="75" spans="4:9" s="13" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="D75" s="5"/>
       <c r="E75" s="7"/>
     </row>
-    <row r="76" spans="4:9" s="15" customFormat="1" ht="14" x14ac:dyDescent="0.2">
+    <row r="76" spans="4:9" s="13" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="D76" s="5"/>
       <c r="E76" s="7"/>
     </row>
-    <row r="77" spans="4:9" s="15" customFormat="1" ht="14" x14ac:dyDescent="0.2">
+    <row r="77" spans="4:9" s="13" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="D77" s="5"/>
       <c r="E77" s="7"/>
     </row>
-    <row r="78" spans="4:9" s="15" customFormat="1" ht="14" x14ac:dyDescent="0.2">
+    <row r="78" spans="4:9" s="13" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="D78" s="5"/>
       <c r="E78" s="7"/>
     </row>
-    <row r="79" spans="4:9" s="15" customFormat="1" ht="14" x14ac:dyDescent="0.2">
+    <row r="79" spans="4:9" s="13" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="D79" s="5"/>
       <c r="E79" s="7"/>
     </row>
-    <row r="80" spans="4:9" s="15" customFormat="1" ht="14" x14ac:dyDescent="0.2">
+    <row r="80" spans="4:9" s="13" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="D80" s="5"/>
       <c r="E80" s="7"/>
     </row>
-    <row r="81" spans="4:5" s="15" customFormat="1" ht="14" x14ac:dyDescent="0.2">
+    <row r="81" spans="4:5" s="13" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="D81" s="5"/>
       <c r="E81" s="7"/>
     </row>
-    <row r="82" spans="4:5" s="15" customFormat="1" ht="14" x14ac:dyDescent="0.2">
+    <row r="82" spans="4:5" s="13" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="D82" s="5"/>
       <c r="E82" s="7"/>
     </row>
-    <row r="83" spans="4:5" s="15" customFormat="1" ht="14" x14ac:dyDescent="0.2">
+    <row r="83" spans="4:5" s="13" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="D83" s="5"/>
       <c r="E83" s="7"/>
     </row>
-    <row r="84" spans="4:5" s="15" customFormat="1" ht="14" x14ac:dyDescent="0.2">
+    <row r="84" spans="4:5" s="13" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="D84" s="5"/>
       <c r="E84" s="7"/>
     </row>
-    <row r="85" spans="4:5" s="15" customFormat="1" ht="14" x14ac:dyDescent="0.2">
+    <row r="85" spans="4:5" s="13" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="D85" s="5"/>
       <c r="E85" s="7"/>
     </row>
-    <row r="86" spans="4:5" s="15" customFormat="1" ht="14" x14ac:dyDescent="0.2">
+    <row r="86" spans="4:5" s="13" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="D86" s="5"/>
       <c r="E86" s="7"/>
     </row>
-    <row r="87" spans="4:5" s="15" customFormat="1" ht="14" x14ac:dyDescent="0.2">
+    <row r="87" spans="4:5" s="13" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="D87" s="5"/>
       <c r="E87" s="7"/>
     </row>
-    <row r="88" spans="4:5" s="15" customFormat="1" ht="14" x14ac:dyDescent="0.2">
+    <row r="88" spans="4:5" s="13" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="D88" s="5"/>
       <c r="E88" s="7"/>
     </row>
-    <row r="89" spans="4:5" s="15" customFormat="1" ht="14" x14ac:dyDescent="0.2">
+    <row r="89" spans="4:5" s="13" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="D89" s="5"/>
       <c r="E89" s="7"/>
     </row>
-    <row r="90" spans="4:5" s="15" customFormat="1" ht="14" x14ac:dyDescent="0.2">
+    <row r="90" spans="4:5" s="13" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="D90" s="5"/>
       <c r="E90" s="7"/>
     </row>
-    <row r="91" spans="4:5" s="15" customFormat="1" ht="14" x14ac:dyDescent="0.2">
+    <row r="91" spans="4:5" s="13" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="D91" s="5"/>
       <c r="E91" s="7"/>
     </row>
-    <row r="92" spans="4:5" s="15" customFormat="1" ht="14" x14ac:dyDescent="0.2">
+    <row r="92" spans="4:5" s="13" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="D92" s="5"/>
       <c r="E92" s="7"/>
     </row>
@@ -2991,257 +3161,257 @@
       <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="115.5" customWidth="1"/>
+    <col min="1" max="1" width="115.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>25</v>
       </c>
@@ -3260,19 +3430,19 @@
       <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>8</v>
       </c>

</xml_diff>

<commit_message>
NPFS after Tcon PC resolution
updated spreadsheets
updated profile with tracked chenges
</commit_message>
<xml_diff>
--- a/FHIR-R4/ITI_Comment_Form-NPFSm_Felhofer.xlsx
+++ b/FHIR-R4/ITI_Comment_Form-NPFSm_Felhofer.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gregorio Canal\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gregorio Canal\Google Drive\IHE\ITI\NPFS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62693DC6-9CAF-4480-A48F-6BA7A8BD2C23}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C95C893-42B2-498F-8306-632E66807824}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,6 +18,7 @@
     <sheet name="PriorityNames" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Comment Form'!$A$5:$J$31</definedName>
     <definedName name="PriorityNames">PriorityNames!$A$1:$A$3</definedName>
     <definedName name="SupplementNames">'Supplement Names'!$A$6:$A$47</definedName>
   </definedNames>
@@ -1150,19 +1151,10 @@
     <t>comment</t>
   </si>
   <si>
-    <t>Discuss</t>
-  </si>
-  <si>
     <t>Resolved</t>
   </si>
   <si>
     <t>used relationship instead of association</t>
-  </si>
-  <si>
-    <t xml:space="preserve">I always intended an NPSFSm file for a  single Privacy Policy and if needed a BPPC template will reference more than one privacy policy file. Either way Type’s cardinality is [1..1] but it is a codeableConcept thus the coding element in it it is repetable. </t>
-  </si>
-  <si>
-    <t>see above</t>
   </si>
   <si>
     <t>Reject</t>
@@ -1176,6 +1168,15 @@
   </si>
   <si>
     <t>Yes it is right. Because it is th same opaque identifier of the binary resource posted.</t>
+  </si>
+  <si>
+    <t>I always intended an NPSFSm file for a  single Privacy Policy and if needed a BPPC template will reference more than one privacy policy file.</t>
+  </si>
+  <si>
+    <t>Drawn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fixed </t>
   </si>
 </sst>
 </file>
@@ -1453,12 +1454,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1473,6 +1468,12 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1814,8 +1815,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B11" zoomScale="88" zoomScaleNormal="88" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1832,31 +1833,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="18" x14ac:dyDescent="0.35">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="24" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
-      <c r="I1" s="19"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
     </row>
     <row r="2" spans="1:10" ht="269.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="23" t="s">
         <v>47</v>
       </c>
-      <c r="B2" s="18"/>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18"/>
-      <c r="G2" s="18"/>
-      <c r="H2" s="18"/>
-      <c r="I2" s="18"/>
-      <c r="J2" s="18"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="23"/>
+      <c r="I2" s="23"/>
+      <c r="J2" s="23"/>
     </row>
     <row r="3" spans="1:10" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="F3" s="14"/>
@@ -1895,10 +1896,10 @@
       <c r="H5" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="I5" s="24" t="s">
+      <c r="I5" s="22" t="s">
         <v>127</v>
       </c>
-      <c r="J5" s="20" t="s">
+      <c r="J5" s="18" t="s">
         <v>128</v>
       </c>
     </row>
@@ -1926,7 +1927,7 @@
       <c r="I6" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="J6" s="21"/>
+      <c r="J6" s="19"/>
     </row>
     <row r="7" spans="1:10" s="13" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
@@ -1952,9 +1953,9 @@
         <v>8</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="J7" s="21"/>
+        <v>129</v>
+      </c>
+      <c r="J7" s="19"/>
     </row>
     <row r="8" spans="1:10" s="13" customFormat="1" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
@@ -1982,9 +1983,9 @@
         <v>8</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="J8" s="21"/>
+        <v>129</v>
+      </c>
+      <c r="J8" s="19"/>
     </row>
     <row r="9" spans="1:10" s="13" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
@@ -2012,9 +2013,9 @@
         <v>8</v>
       </c>
       <c r="I9" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="J9" s="21"/>
+        <v>129</v>
+      </c>
+      <c r="J9" s="19"/>
     </row>
     <row r="10" spans="1:10" s="13" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
@@ -2042,9 +2043,9 @@
         <v>8</v>
       </c>
       <c r="I10" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="J10" s="21"/>
+        <v>129</v>
+      </c>
+      <c r="J10" s="19"/>
     </row>
     <row r="11" spans="1:10" s="13" customFormat="1" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
@@ -2072,9 +2073,9 @@
         <v>8</v>
       </c>
       <c r="I11" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="J11" s="21"/>
+        <v>129</v>
+      </c>
+      <c r="J11" s="19"/>
     </row>
     <row r="12" spans="1:10" s="13" customFormat="1" ht="79.2" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
@@ -2102,9 +2103,9 @@
         <v>8</v>
       </c>
       <c r="I12" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="J12" s="21"/>
+        <v>129</v>
+      </c>
+      <c r="J12" s="19"/>
     </row>
     <row r="13" spans="1:10" s="13" customFormat="1" ht="79.2" x14ac:dyDescent="0.3">
       <c r="A13" s="6" t="s">
@@ -2130,10 +2131,10 @@
         <v>8</v>
       </c>
       <c r="I13" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="J13" s="19" t="s">
         <v>130</v>
-      </c>
-      <c r="J13" s="21" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="14" spans="1:10" s="13" customFormat="1" ht="39.6" x14ac:dyDescent="0.3">
@@ -2162,9 +2163,9 @@
         <v>8</v>
       </c>
       <c r="I14" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="J14" s="21"/>
+        <v>129</v>
+      </c>
+      <c r="J14" s="19"/>
     </row>
     <row r="15" spans="1:10" s="13" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A15" s="6" t="s">
@@ -2192,9 +2193,9 @@
         <v>8</v>
       </c>
       <c r="I15" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="J15" s="21"/>
+        <v>129</v>
+      </c>
+      <c r="J15" s="19"/>
     </row>
     <row r="16" spans="1:10" s="13" customFormat="1" ht="66" x14ac:dyDescent="0.3">
       <c r="A16" s="6" t="s">
@@ -2222,9 +2223,9 @@
         <v>8</v>
       </c>
       <c r="I16" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="J16" s="21"/>
+        <v>129</v>
+      </c>
+      <c r="J16" s="19"/>
     </row>
     <row r="17" spans="1:10" s="13" customFormat="1" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
@@ -2254,7 +2255,7 @@
       <c r="I17" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="J17" s="21"/>
+      <c r="J17" s="19"/>
     </row>
     <row r="18" spans="1:10" s="13" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
@@ -2282,9 +2283,9 @@
         <v>8</v>
       </c>
       <c r="I18" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="J18" s="21"/>
+        <v>129</v>
+      </c>
+      <c r="J18" s="19"/>
     </row>
     <row r="19" spans="1:10" s="13" customFormat="1" ht="211.2" x14ac:dyDescent="0.3">
       <c r="A19" s="6" t="s">
@@ -2312,10 +2313,10 @@
         <v>9</v>
       </c>
       <c r="I19" s="4" t="s">
-        <v>129</v>
-      </c>
-      <c r="J19" s="22" t="s">
-        <v>132</v>
+        <v>136</v>
+      </c>
+      <c r="J19" s="20" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="20" spans="1:10" s="13" customFormat="1" ht="26.4" x14ac:dyDescent="0.3">
@@ -2346,8 +2347,8 @@
       <c r="I20" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="J20" s="21" t="s">
-        <v>133</v>
+      <c r="J20" s="19" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="21" spans="1:10" s="13" customFormat="1" ht="82.8" x14ac:dyDescent="0.3">
@@ -2368,10 +2369,10 @@
       <c r="G21" s="6"/>
       <c r="H21" s="6"/>
       <c r="I21" s="4" t="s">
-        <v>134</v>
-      </c>
-      <c r="J21" s="21" t="s">
-        <v>135</v>
+        <v>131</v>
+      </c>
+      <c r="J21" s="19" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="22" spans="1:10" s="13" customFormat="1" ht="92.4" x14ac:dyDescent="0.3">
@@ -2398,10 +2399,10 @@
         <v>9</v>
       </c>
       <c r="I22" s="4" t="s">
-        <v>129</v>
-      </c>
-      <c r="J22" s="21" t="s">
         <v>136</v>
+      </c>
+      <c r="J22" s="19" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="23" spans="1:10" s="13" customFormat="1" ht="52.8" x14ac:dyDescent="0.3">
@@ -2430,9 +2431,9 @@
         <v>8</v>
       </c>
       <c r="I23" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="J23" s="21"/>
+        <v>129</v>
+      </c>
+      <c r="J23" s="19"/>
     </row>
     <row r="24" spans="1:10" s="13" customFormat="1" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A24" s="6" t="s">
@@ -2458,10 +2459,10 @@
         <v>8</v>
       </c>
       <c r="I24" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="J24" s="21" t="s">
-        <v>137</v>
+        <v>129</v>
+      </c>
+      <c r="J24" s="19" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="25" spans="1:10" s="13" customFormat="1" ht="52.8" x14ac:dyDescent="0.3">
@@ -2490,9 +2491,9 @@
         <v>8</v>
       </c>
       <c r="I25" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="J25" s="21"/>
+        <v>129</v>
+      </c>
+      <c r="J25" s="19"/>
     </row>
     <row r="26" spans="1:10" s="13" customFormat="1" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A26" s="6" t="s">
@@ -2520,9 +2521,9 @@
         <v>8</v>
       </c>
       <c r="I26" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="J26" s="21"/>
+        <v>129</v>
+      </c>
+      <c r="J26" s="19"/>
     </row>
     <row r="27" spans="1:10" s="13" customFormat="1" ht="79.2" x14ac:dyDescent="0.3">
       <c r="A27" s="6" t="s">
@@ -2550,9 +2551,9 @@
         <v>8</v>
       </c>
       <c r="I27" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="J27" s="21"/>
+        <v>129</v>
+      </c>
+      <c r="J27" s="19"/>
     </row>
     <row r="28" spans="1:10" s="13" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A28" s="6" t="s">
@@ -2580,9 +2581,9 @@
         <v>8</v>
       </c>
       <c r="I28" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="J28" s="21"/>
+        <v>129</v>
+      </c>
+      <c r="J28" s="19"/>
     </row>
     <row r="29" spans="1:10" s="13" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A29" s="6" t="s">
@@ -2610,9 +2611,9 @@
         <v>8</v>
       </c>
       <c r="I29" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="J29" s="21"/>
+        <v>129</v>
+      </c>
+      <c r="J29" s="19"/>
     </row>
     <row r="30" spans="1:10" s="13" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
@@ -2640,9 +2641,9 @@
         <v>8</v>
       </c>
       <c r="I30" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="J30" s="21"/>
+        <v>129</v>
+      </c>
+      <c r="J30" s="19"/>
     </row>
     <row r="31" spans="1:10" s="13" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A31" s="6" t="s">
@@ -2668,9 +2669,9 @@
         <v>8</v>
       </c>
       <c r="I31" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="J31" s="21"/>
+        <v>129</v>
+      </c>
+      <c r="J31" s="19"/>
     </row>
     <row r="32" spans="1:10" s="13" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A32" s="12"/>
@@ -2682,7 +2683,7 @@
       <c r="G32" s="6"/>
       <c r="H32" s="6"/>
       <c r="I32" s="5"/>
-      <c r="J32" s="23"/>
+      <c r="J32" s="21"/>
     </row>
     <row r="33" spans="1:9" s="13" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A33" s="12"/>
@@ -3124,6 +3125,7 @@
       <c r="E92" s="7"/>
     </row>
   </sheetData>
+  <autoFilter ref="A5:J31" xr:uid="{2F18CC7D-B279-4811-B7C3-A0A40DBF3D99}"/>
   <mergeCells count="2">
     <mergeCell ref="A2:J2"/>
     <mergeCell ref="A1:I1"/>

</xml_diff>